<commit_message>
Xlsx modified, tests working and completed
</commit_message>
<xml_diff>
--- a/research/comparison.xlsx
+++ b/research/comparison.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="13">
   <si>
     <t xml:space="preserve">Doc_ID</t>
   </si>
@@ -212,16 +212,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="7" min="1" style="1" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.8056680161943"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.8178137651822"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -497,176 +497,176 @@
       <c r="G12" s="5"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="n">
-        <v>1210</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="D13" s="6" t="n">
+    <row r="13" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="n">
+        <v>1210</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>300</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="n">
+        <v>1210</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>300</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="n">
+        <v>1210</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>300</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>60</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="n">
+        <v>1210</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>300</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="n">
+        <v>1210</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>300</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="n">
+        <v>1210</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="D18" s="6" t="n">
         <v>50</v>
       </c>
-      <c r="E13" s="6" t="n">
-        <v>40</v>
-      </c>
-      <c r="F13" s="6" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="7" t="s">
+      <c r="E18" s="6" t="n">
+        <v>40</v>
+      </c>
+      <c r="F18" s="6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G18" s="6"/>
+      <c r="H18" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
-        <v>1210</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="D14" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="E14" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="F14" s="3" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
-        <v>1210</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="D15" s="3" t="n">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="n">
+        <v>1210</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="D19" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="n">
+        <v>1210</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="D20" s="3" t="n">
         <v>150</v>
-      </c>
-      <c r="E15" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="F15" s="3" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
-        <v>1210</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="D16" s="3" t="n">
-        <v>200</v>
-      </c>
-      <c r="E16" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="F16" s="3" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
-        <v>1210</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="D17" s="3" t="n">
-        <v>250</v>
-      </c>
-      <c r="E17" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="F17" s="3" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="n">
-        <v>1210</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="5" t="n">
-        <v>100</v>
-      </c>
-      <c r="D18" s="5" t="n">
-        <v>300</v>
-      </c>
-      <c r="E18" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F18" s="5" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="n">
-        <v>1210</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="6" t="n">
-        <v>50</v>
-      </c>
-      <c r="D19" s="6" t="n">
-        <v>300</v>
-      </c>
-      <c r="E19" s="6" t="n">
-        <v>40</v>
-      </c>
-      <c r="F19" s="6" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
-        <v>1210</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="D20" s="3" t="n">
-        <v>300</v>
       </c>
       <c r="E20" s="3" t="n">
         <v>40</v>
@@ -677,7 +677,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="n">
         <v>1210</v>
       </c>
@@ -685,10 +685,10 @@
         <v>8</v>
       </c>
       <c r="C21" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="D21" s="3" t="n">
         <v>200</v>
-      </c>
-      <c r="D21" s="3" t="n">
-        <v>300</v>
       </c>
       <c r="E21" s="3" t="n">
         <v>40</v>
@@ -699,34 +699,146 @@
       <c r="G21" s="3"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="n">
-        <v>1210</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="5" t="n">
-        <v>300</v>
-      </c>
-      <c r="D22" s="5" t="n">
-        <v>300</v>
-      </c>
-      <c r="E22" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F22" s="5" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="G22" s="5"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="n">
+        <v>1210</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="D22" s="3" t="n">
+        <v>250</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G22" s="3"/>
       <c r="H22" s="7"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="n">
+        <v>1210</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>300</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G23" s="5"/>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="n">
+        <v>1210</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="D24" s="6" t="n">
+        <v>300</v>
+      </c>
+      <c r="E24" s="6" t="n">
+        <v>40</v>
+      </c>
+      <c r="F24" s="6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G24" s="6"/>
+      <c r="H24" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="n">
+        <v>1210</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>300</v>
+      </c>
+      <c r="E25" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="F25" s="3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G25" s="3"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="n">
+        <v>1210</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="3" t="n">
+        <v>200</v>
+      </c>
+      <c r="D26" s="3" t="n">
+        <v>300</v>
+      </c>
+      <c r="E26" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="F26" s="3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G26" s="3"/>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="n">
+        <v>1210</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="5" t="n">
+        <v>300</v>
+      </c>
+      <c r="D27" s="5" t="n">
+        <v>300</v>
+      </c>
+      <c r="E27" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="F27" s="5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G27" s="5"/>
+      <c r="H27" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="H2:H7"/>
     <mergeCell ref="H8:H12"/>
-    <mergeCell ref="H13:H18"/>
-    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="H18:H23"/>
+    <mergeCell ref="H24:H27"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>